<commit_message>
Cleaning up project and eliminating unused source.
</commit_message>
<xml_diff>
--- a/PipeDiameters.xlsx
+++ b/PipeDiameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandt/PycharmProjects/SimulinkInterface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412D92EB-778C-3549-814B-D419A7D1FB87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BE305D-F97F-2347-B71B-6E02FE684455}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1380" yWindow="-17780" windowWidth="28800" windowHeight="16020" xr2:uid="{702B85D2-345D-C74F-B174-48AF370D3B37}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{702B85D2-345D-C74F-B174-48AF370D3B37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FF64F3-ED1E-8749-8419-DAB53507EAE2}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" ref="B21:B31" si="3">(A21 * 1000000) / ($E$20 * 1000 * $E$21)</f>
+        <f t="shared" ref="B21:B32" si="3">(A21 * 1000000) / ($E$20 * 1000 * $E$21)</f>
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -882,6 +882,15 @@
       <c r="B31" s="3">
         <f t="shared" si="3"/>
         <v>146.98209023230518</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2600</v>
+      </c>
+      <c r="B32" s="3">
+        <f t="shared" si="3"/>
+        <v>382.1534346039935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated file naming convention in logger
</commit_message>
<xml_diff>
--- a/PipeDiameters.xlsx
+++ b/PipeDiameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandt/PycharmProjects/SimulinkInterface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BE305D-F97F-2347-B71B-6E02FE684455}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C9579E-76ED-1946-ACAE-D061265006AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{702B85D2-345D-C74F-B174-48AF370D3B37}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{702B85D2-345D-C74F-B174-48AF370D3B37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -462,18 +462,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FF64F3-ED1E-8749-8419-DAB53507EAE2}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.5" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -784,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" ref="B21:B32" si="3">(A21 * 1000000) / ($E$20 * 1000 * $E$21)</f>
+        <f t="shared" ref="B21:B34" si="3">(A21 * 1000000) / ($E$20 * 1000 * $E$21)</f>
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -885,12 +885,30 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="2">
         <v>2600</v>
       </c>
       <c r="B32" s="3">
         <f t="shared" si="3"/>
         <v>382.1534346039935</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>2800</v>
+      </c>
+      <c r="B33" s="3">
+        <f t="shared" si="3"/>
+        <v>411.54985265045457</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>2900</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" si="3"/>
+        <v>426.24806167368507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>